<commit_message>
Improved Introduction section on motivation for this plugin and added example.
</commit_message>
<xml_diff>
--- a/src/test/resources/spec/concordion/ext/excel/ExcelConcordionTutorial.xlsx
+++ b/src/test/resources/spec/concordion/ext/excel/ExcelConcordionTutorial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25280" windowHeight="15320" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25280" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Rob Moffat</author>
   </authors>
   <commentList>
-    <comment ref="A4" authorId="0">
+    <comment ref="A11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,8 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Rob Moffat:</t>
+          <t xml:space="preserve">Rob Moffat:
+</t>
         </r>
         <r>
           <rPr>
@@ -50,11 +51,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-html-tag="pre"</t>
+(table)concordion:execute="#result = calculateResult(#a, #b, #c)"
+concordion:set="#a"</t>
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,11 +76,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-concordion:assertEquals="blah()"</t>
+concordion:set="#b"</t>
         </r>
       </text>
     </comment>
-    <comment ref="A12" authorId="0">
+    <comment ref="C11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +100,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-html-tag="pre"</t>
+concordion:set="#c"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rob Moffat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+concordion:assertEquals="#result"</t>
         </r>
       </text>
     </comment>
@@ -107,6 +133,88 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Rob Moffat</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rob Moffat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+html-tag="pre"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rob Moffat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+concordion:assertEquals="blah()"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rob Moffat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+html-tag="pre"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Rob Moffat</author>
@@ -164,7 +272,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Rob Moffat</author>
@@ -271,7 +379,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Rob Moffat</author>
@@ -306,7 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>The Concordion Excel parser contains functionality for converting tests written in Excel format (like this one) into HTML format for Concordion to process.</t>
   </si>
@@ -503,6 +611,33 @@
   </si>
   <si>
     <t>To add a cell comment, right-click the cell and select "Insert Comment"</t>
+  </si>
+  <si>
+    <t>Let's say you were writing a formula, and you wanted to write an acceptance test for it.  You might start by including some examples like so:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating tables of data in HTML format for Concordion can be a bit of a faff.  </t>
+  </si>
+  <si>
+    <t>However, the Excel GUI as it stands is very good at tables.  If you have people on your team without HTML skills (say, business analysts) they may find putting tests together in Excel a bit easier than in HTML.</t>
+  </si>
+  <si>
+    <t>Not only might this be easier to do and less error-prone than the pencil-and-paper way, but it serves as a demonstration to the developers of how the formula should work.</t>
+  </si>
+  <si>
+    <t>Rather than sitting down with a piece of paper and working out all the values in the "Result" column, you might be able to save time by writing an Excel formula for doing it</t>
   </si>
 </sst>
 </file>
@@ -601,7 +736,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -616,6 +751,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
@@ -632,7 +775,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -642,11 +785,19 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -655,6 +806,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A11:D15" totalsRowShown="0">
+  <autoFilter ref="A11:D15"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="A "/>
+    <tableColumn id="2" name="B"/>
+    <tableColumn id="3" name="C"/>
+    <tableColumn id="4" name="Result">
+      <calculatedColumnFormula>A12*B12+C12</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A4:C7" totalsRowShown="0">
   <autoFilter ref="A4:C7"/>
   <tableColumns count="3">
@@ -666,7 +832,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:C5" totalsRowShown="0">
   <autoFilter ref="A3:C5"/>
   <tableColumns count="3">
@@ -999,37 +1165,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f>A12*B12+C12</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>A13*B13+C13</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>A14*B14+C14</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f>A15*B15+C15</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="5" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1170,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -1307,7 +1577,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Added unit tests, removed tutorial from this project, modified table process.
</commit_message>
<xml_diff>
--- a/src/test/resources/spec/concordion/ext/excel/ExcelConcordionTutorial.xlsx
+++ b/src/test/resources/spec/concordion/ext/excel/ExcelConcordionTutorial.xlsx
@@ -644,6 +644,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -761,7 +764,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -774,6 +777,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -800,7 +804,11 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -812,7 +820,7 @@
     <tableColumn id="1" name="A "/>
     <tableColumn id="2" name="B"/>
     <tableColumn id="3" name="C"/>
-    <tableColumn id="4" name="Result">
+    <tableColumn id="4" name="Result" dataDxfId="0">
       <calculatedColumnFormula>A12*B12+C12</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1169,7 +1177,7 @@
   <dimension ref="A2:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D12" sqref="D12:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1218,7 +1226,7 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <f>A12*B12+C12</f>
         <v>11</v>
       </c>
@@ -1233,7 +1241,7 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
         <f>A13*B13+C13</f>
         <v>19</v>
       </c>
@@ -1248,7 +1256,7 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <f>A14*B14+C14</f>
         <v>26</v>
       </c>
@@ -1263,7 +1271,7 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="8">
         <f>A15*B15+C15</f>
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added in hidden column code.  Currently failing
</commit_message>
<xml_diff>
--- a/src/test/resources/spec/concordion/ext/excel/ExcelConcordionTutorial.xlsx
+++ b/src/test/resources/spec/concordion/ext/excel/ExcelConcordionTutorial.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25280" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="3700" yWindow="4260" windowWidth="25280" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -1177,10 +1177,13 @@
   <dimension ref="A2:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:D15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" t="s">

</xml_diff>